<commit_message>
table composante: ajout de code_uai_composante
</commit_message>
<xml_diff>
--- a/data-raw/data/Composante.xlsx
+++ b/data-raw/data/Composante.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="161">
   <si>
     <t>Composante (code)</t>
   </si>
@@ -24,6 +24,9 @@
     <t>Composante - Type (code)</t>
   </si>
   <si>
+    <t>Code RNE composante</t>
+  </si>
+  <si>
     <t>AL1</t>
   </si>
   <si>
@@ -42,9 +45,15 @@
     <t>LOC</t>
   </si>
   <si>
+    <t>0811255Z</t>
+  </si>
+  <si>
     <t>AL3</t>
   </si>
   <si>
+    <t>0811198M</t>
+  </si>
+  <si>
     <t>ALB</t>
   </si>
   <si>
@@ -60,6 +69,9 @@
     <t>UFR</t>
   </si>
   <si>
+    <t>0311621U</t>
+  </si>
+  <si>
     <t>AUC</t>
   </si>
   <si>
@@ -69,6 +81,9 @@
     <t>32013</t>
   </si>
   <si>
+    <t>0320691C</t>
+  </si>
+  <si>
     <t>BIO</t>
   </si>
   <si>
@@ -84,6 +99,9 @@
     <t>81065</t>
   </si>
   <si>
+    <t>0811199N</t>
+  </si>
+  <si>
     <t>CHI</t>
   </si>
   <si>
@@ -96,12 +114,18 @@
     <t>DENTAIRE</t>
   </si>
   <si>
+    <t>0311533Y</t>
+  </si>
+  <si>
     <t>DEU</t>
   </si>
   <si>
     <t>DEUG</t>
   </si>
   <si>
+    <t>0312533K</t>
+  </si>
+  <si>
     <t>EEA</t>
   </si>
   <si>
@@ -111,9 +135,15 @@
     <t>FCA</t>
   </si>
   <si>
+    <t>0312499Y</t>
+  </si>
+  <si>
     <t>FSI</t>
   </si>
   <si>
+    <t>0312837R</t>
+  </si>
+  <si>
     <t>INF</t>
   </si>
   <si>
@@ -129,24 +159,36 @@
     <t>IUP</t>
   </si>
   <si>
+    <t>0312452X</t>
+  </si>
+  <si>
     <t>IU2</t>
   </si>
   <si>
     <t>IUP GMP</t>
   </si>
   <si>
+    <t>0312437F</t>
+  </si>
+  <si>
     <t>IU3</t>
   </si>
   <si>
     <t>IUP GCI</t>
   </si>
   <si>
+    <t>0312438G</t>
+  </si>
+  <si>
     <t>IU4</t>
   </si>
   <si>
     <t>IUP ISI</t>
   </si>
   <si>
+    <t>0312586T</t>
+  </si>
+  <si>
     <t>IU5</t>
   </si>
   <si>
@@ -159,24 +201,36 @@
     <t>IUP MIAGE</t>
   </si>
   <si>
+    <t>0312441K</t>
+  </si>
+  <si>
     <t>IU7</t>
   </si>
   <si>
     <t>IUP STRI</t>
   </si>
   <si>
+    <t>0312443M</t>
+  </si>
+  <si>
     <t>IU8</t>
   </si>
   <si>
     <t>IUP GEO SC</t>
   </si>
   <si>
+    <t>0312451W</t>
+  </si>
+  <si>
     <t>IU9</t>
   </si>
   <si>
     <t>IUP TMM</t>
   </si>
   <si>
+    <t>0312436E</t>
+  </si>
+  <si>
     <t>IUA</t>
   </si>
   <si>
@@ -186,6 +240,9 @@
     <t>65440</t>
   </si>
   <si>
+    <t>0651025L</t>
+  </si>
+  <si>
     <t>IUB</t>
   </si>
   <si>
@@ -198,6 +255,9 @@
     <t>IUP SPORT</t>
   </si>
   <si>
+    <t>0312585S</t>
+  </si>
+  <si>
     <t>IUD</t>
   </si>
   <si>
@@ -210,6 +270,9 @@
     <t>IUP I.E.R.</t>
   </si>
   <si>
+    <t>0312587U</t>
+  </si>
+  <si>
     <t>IUF</t>
   </si>
   <si>
@@ -222,18 +285,27 @@
     <t>IUP ISME</t>
   </si>
   <si>
+    <t>0312343D</t>
+  </si>
+  <si>
     <t>IUT</t>
   </si>
   <si>
     <t>IUT A</t>
   </si>
   <si>
+    <t>0311086M</t>
+  </si>
+  <si>
     <t>LAN</t>
   </si>
   <si>
     <t>LANG.VIV.</t>
   </si>
   <si>
+    <t>0311535A</t>
+  </si>
+  <si>
     <t>LVG</t>
   </si>
   <si>
@@ -255,6 +327,9 @@
     <t>MIG</t>
   </si>
   <si>
+    <t>0311806V</t>
+  </si>
+  <si>
     <t>MPS</t>
   </si>
   <si>
@@ -267,15 +342,24 @@
     <t>INS</t>
   </si>
   <si>
+    <t>0310131Z</t>
+  </si>
+  <si>
     <t>PCA</t>
   </si>
   <si>
+    <t>0311804T</t>
+  </si>
+  <si>
     <t>PHA</t>
   </si>
   <si>
     <t>PHARMACIE</t>
   </si>
   <si>
+    <t>0311526R</t>
+  </si>
+  <si>
     <t>PHY</t>
   </si>
   <si>
@@ -294,12 +378,18 @@
     <t>PURPAN</t>
   </si>
   <si>
+    <t>0311528T</t>
+  </si>
+  <si>
     <t>RAN</t>
   </si>
   <si>
     <t>RANGUEIL</t>
   </si>
   <si>
+    <t>0311527S</t>
+  </si>
+  <si>
     <t>ROD</t>
   </si>
   <si>
@@ -309,18 +399,27 @@
     <t>12202</t>
   </si>
   <si>
+    <t>0121439Z</t>
+  </si>
+  <si>
     <t>SCA</t>
   </si>
   <si>
     <t>SCUAPS</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>SCU</t>
   </si>
   <si>
     <t>scol.centr</t>
   </si>
   <si>
+    <t>0311384L</t>
+  </si>
+  <si>
     <t>SHN</t>
   </si>
   <si>
@@ -330,15 +429,24 @@
     <t>TARBES DG</t>
   </si>
   <si>
+    <t>0651001K</t>
+  </si>
+  <si>
     <t>SVT</t>
   </si>
   <si>
+    <t>0311805U</t>
+  </si>
+  <si>
     <t>TAR</t>
   </si>
   <si>
     <t>IUT TARBES</t>
   </si>
   <si>
+    <t>0650583F</t>
+  </si>
+  <si>
     <t>UTT</t>
   </si>
   <si>
@@ -346,6 +454,9 @@
   </si>
   <si>
     <t>COM</t>
+  </si>
+  <si>
+    <t>0312877J</t>
   </si>
   <si>
     <t>Composante - Commune (lib.)</t>
@@ -468,11 +579,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:F57"/>
   <cols>
     <col min="1" max="1" width="1.0008" customWidth="1"/>
-    <col min="2" max="5" width="10.7163133333333" customWidth="1"/>
-    <col min="6" max="6" width="4.67767866666667" customWidth="1"/>
+    <col min="2" max="6" width="10.7163133333333" customWidth="1"/>
+    <col min="7" max="7" width="4.67767866666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="58.663" customHeight="1"/>
@@ -489,749 +600,888 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B22" s="3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B26" s="3" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B27" s="3" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B29" s="3" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B30" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B31" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B34" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B35" s="3" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>70</v>
+        <v>92</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B36" s="3" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B37" s="3" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B38" s="3" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B39" s="3" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B40" s="3" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>84</v>
+        <v>109</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B43" s="3" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B44" s="3" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B45" s="3" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B46" s="3" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B47" s="3" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B48" s="3" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B49" s="3" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B50" s="3" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B51" s="3" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B52" s="3" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B53" s="3" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="54" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B54" s="3" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B55" s="3" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>70</v>
+        <v>92</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B56" s="3" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3" t="s">
-        <v>111</v>
+        <v>147</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
@@ -1256,55 +1506,55 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="11.1993" customHeight="1">
@@ -1333,63 +1583,63 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>

</xml_diff>